<commit_message>
Tilføjede noget til et WIP excel
</commit_message>
<xml_diff>
--- a/Documentation/Danske Personvogne.xlsx
+++ b/Documentation/Danske Personvogne.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\1993m\Documents\GitHub\Pak128.Nordic\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56021B0-F54B-460C-9C84-84FA15410D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCE3149-ADDF-4395-89A3-A47181AAA69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Forklaring" sheetId="2" r:id="rId1"/>
     <sheet name="Danske personvogne" sheetId="1" r:id="rId2"/>
+    <sheet name="Danske damplokomotiver" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="218">
   <si>
     <t>name=BR-390FrontCab</t>
   </si>
@@ -217,12 +218,12 @@
     <t>sound</t>
   </si>
   <si>
-    <t>can_lead_from_rear</t>
-  </si>
-  <si>
     <t>bidirectional</t>
   </si>
   <si>
+    <t>is_tilting</t>
+  </si>
+  <si>
     <t>min_loading_tiime</t>
   </si>
   <si>
@@ -247,9 +248,6 @@
     <t>air_resistance</t>
   </si>
   <si>
-    <t>https://simutrans-germany.com/wiki/wiki/en_VehicleDef#Constraint_Parameters</t>
-  </si>
-  <si>
     <t>Constraint[Prev]</t>
   </si>
   <si>
@@ -257,9 +255,6 @@
   </si>
   <si>
     <t>liverytype</t>
-  </si>
-  <si>
-    <t>type af objekt. For køretøjer altiv =vehicle</t>
   </si>
   <si>
     <t>Navnet på toget. Ikke det, der vises for spilleren</t>
@@ -451,6 +446,9 @@
     <t xml:space="preserve">Hvilket niveau af catering, køretøjet har (mellem 0-5) for passagerkøretøjer. For postvogne bliver det til en postbureauvogn. </t>
   </si>
   <si>
+    <t>mixed_load_prohibition</t>
+  </si>
+  <si>
     <t>mixed_load_prohibition=1</t>
   </si>
   <si>
@@ -602,13 +600,122 @@
   </si>
   <si>
     <t>Samme syntax som "EmptyImage", men for læssede køretøjer</t>
+  </si>
+  <si>
+    <t>https://forum.simutrans.com/index.php/topic,15174.0.html</t>
+  </si>
+  <si>
+    <t>https://simutrans-germany.com/wiki/wiki/en_VehicleDef</t>
+  </si>
+  <si>
+    <t>type af objekt. For køretøjer altid =vehicle</t>
+  </si>
+  <si>
+    <t>vehicle</t>
+  </si>
+  <si>
+    <t>track</t>
+  </si>
+  <si>
+    <t>ex</t>
+  </si>
+  <si>
+    <t>payload</t>
+  </si>
+  <si>
+    <t>air_resistance is a coefficient to calculate drag force: F= speed^2 * air_resistance</t>
+  </si>
+  <si>
+    <t>available_only_as_upgrade</t>
+  </si>
+  <si>
+    <t>upgrade_price</t>
+  </si>
+  <si>
+    <t>Human name</t>
+  </si>
+  <si>
+    <t>SJS 1./2.</t>
+  </si>
+  <si>
+    <t>passagiere</t>
+  </si>
+  <si>
+    <t>SJS 3. kl</t>
+  </si>
+  <si>
+    <t>SJS post</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>SJS Aa</t>
+  </si>
+  <si>
+    <t>SJS Ba</t>
+  </si>
+  <si>
+    <t>SJS Ca</t>
+  </si>
+  <si>
+    <t>Odin</t>
+  </si>
+  <si>
+    <t>steam</t>
+  </si>
+  <si>
+    <t>OdinTender</t>
+  </si>
+  <si>
+    <t>Thor</t>
+  </si>
+  <si>
+    <t>ThorTender</t>
+  </si>
+  <si>
+    <t>Skirner</t>
+  </si>
+  <si>
+    <t>Steam</t>
+  </si>
+  <si>
+    <t>Roeskilde</t>
+  </si>
+  <si>
+    <t>Thor, Skirner, Roeskilde</t>
+  </si>
+  <si>
+    <t>H. C. Ørsted</t>
+  </si>
+  <si>
+    <t>H. C. Ørsted Tender</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>E-klassen</t>
+  </si>
+  <si>
+    <t>SJS Bogiepost (nr 81-84)</t>
+  </si>
+  <si>
+    <t>SJS Db</t>
+  </si>
+  <si>
+    <t>SJS Ab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="171" formatCode="0&quot; km/t&quot;"/>
+    <numFmt numFmtId="173" formatCode="0.0&quot; t&quot;"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -620,6 +727,14 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -642,10 +757,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -655,8 +771,19 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -937,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDAB390C-EB3C-47C0-B1C9-8DBD38503A44}">
   <dimension ref="A1:R80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,7 +1078,7 @@
         <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -959,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -967,21 +1094,21 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -989,10 +1116,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1000,21 +1127,24 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B7" t="s">
+        <v>188</v>
+      </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1022,10 +1152,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1033,7 +1163,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>1</v>
@@ -1044,10 +1174,10 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1055,29 +1185,29 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R13" s="2"/>
     </row>
@@ -1092,135 +1222,171 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B17" t="s">
+        <v>188</v>
+      </c>
       <c r="C17" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B18" t="s">
+        <v>188</v>
+      </c>
       <c r="C18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B19" t="s">
+        <v>188</v>
+      </c>
       <c r="C19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B20" t="s">
+        <v>188</v>
+      </c>
       <c r="C20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
+        <v>188</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B22" t="s">
+        <v>188</v>
+      </c>
       <c r="C22" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
+      </c>
+      <c r="B23" t="s">
+        <v>188</v>
       </c>
       <c r="C23" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B25" t="s">
+        <v>188</v>
+      </c>
       <c r="C25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B26" t="s">
+        <v>188</v>
+      </c>
       <c r="C26" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B29" t="s">
+        <v>188</v>
+      </c>
       <c r="C29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1228,23 +1394,29 @@
         <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" t="s">
+        <v>188</v>
+      </c>
+      <c r="C34" t="s">
         <v>112</v>
-      </c>
-      <c r="C34" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" t="s">
+        <v>188</v>
+      </c>
+      <c r="C35" t="s">
         <v>113</v>
-      </c>
-      <c r="C35" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1252,448 +1424,2657 @@
         <v>25</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B37" t="s">
+        <v>188</v>
+      </c>
       <c r="C37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B39" t="s">
+        <v>188</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B40" t="s">
+        <v>188</v>
+      </c>
+      <c r="C40" t="s">
         <v>137</v>
-      </c>
-      <c r="C40" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" t="s">
+        <v>188</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" t="s">
+        <v>188</v>
+      </c>
+      <c r="C42" t="s">
         <v>141</v>
-      </c>
-      <c r="C42" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B43" t="s">
+        <v>188</v>
+      </c>
+      <c r="C43" t="s">
         <v>143</v>
-      </c>
-      <c r="C43" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B44" t="s">
+        <v>188</v>
+      </c>
       <c r="C44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="B45" t="s">
+        <v>188</v>
+      </c>
       <c r="C45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="B46" t="s">
+        <v>188</v>
+      </c>
       <c r="C46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B47" t="s">
+        <v>188</v>
+      </c>
       <c r="C47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="B48" t="s">
+        <v>188</v>
+      </c>
       <c r="C48" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="B49" t="s">
+        <v>188</v>
+      </c>
       <c r="C49" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="B50" t="s">
+        <v>188</v>
+      </c>
+      <c r="C50" t="s">
         <v>149</v>
       </c>
-      <c r="C50" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="B51" t="s">
+        <v>188</v>
+      </c>
       <c r="C51" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="J51" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C53" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C55" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B57" t="s">
+        <v>188</v>
+      </c>
+      <c r="C57" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C57" t="s">
+      <c r="B58" t="s">
+        <v>188</v>
+      </c>
+      <c r="C58" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C58" t="s">
+      <c r="B59" t="s">
+        <v>188</v>
+      </c>
+      <c r="C59" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C59" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="C61" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C61" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="C62" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C63" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="C64" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C65" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C66" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
+      </c>
+      <c r="B70" t="s">
+        <v>188</v>
       </c>
       <c r="C70" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
+      </c>
+      <c r="B71" t="s">
+        <v>188</v>
       </c>
       <c r="C71" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
+      </c>
+      <c r="B72" t="s">
+        <v>188</v>
       </c>
       <c r="C72" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
+      </c>
+      <c r="B73" t="s">
+        <v>188</v>
       </c>
       <c r="C73" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
+      </c>
+      <c r="B74" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
+      </c>
+      <c r="B75" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
+      </c>
+      <c r="B76" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
+      </c>
+      <c r="B77" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C79" t="s">
         <v>181</v>
-      </c>
-      <c r="C79" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C80" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="R17" r:id="rId1" xr:uid="{2E8022C6-8143-4EAD-9403-920444866EAF}"/>
+    <hyperlink ref="R18" r:id="rId2" xr:uid="{99E61DFA-6847-470C-92F2-C80C99D7FE2A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR51"/>
+  <dimension ref="A1:AS170"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.140625" style="8"/>
+    <col min="14" max="14" width="9.140625" style="10"/>
+    <col min="27" max="27" width="9.140625" style="9"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
       <c r="B1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
+      <c r="D1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="P1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF1" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" s="8">
+        <v>50</v>
+      </c>
+      <c r="F2">
+        <v>1847</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>187</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="S2">
+        <v>32</v>
+      </c>
+      <c r="T2">
+        <v>12</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="9">
+        <v>10.6</v>
+      </c>
+      <c r="AB2">
+        <v>3</v>
+      </c>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" s="8">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>1847</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="R3">
+        <v>60</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="9">
+        <v>9.6</v>
+      </c>
+      <c r="AB3">
+        <v>3</v>
+      </c>
+      <c r="AG3" s="3"/>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" s="8">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>1847</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>187</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="P4">
+        <v>1000</v>
+      </c>
+      <c r="AA4" s="9">
+        <v>12.5</v>
+      </c>
+      <c r="AB4">
+        <v>3</v>
+      </c>
+      <c r="AG4" s="3"/>
+      <c r="AH4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F5">
+        <v>1863</v>
+      </c>
+      <c r="J5" t="s">
+        <v>187</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="S5">
+        <v>24</v>
+      </c>
+      <c r="T5">
+        <v>7</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="9">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="AB5">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="3"/>
+      <c r="AH5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" t="s">
+        <v>200</v>
+      </c>
+      <c r="F6">
+        <v>1865</v>
+      </c>
+      <c r="J6" t="s">
+        <v>187</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="R6">
+        <v>30</v>
+      </c>
+      <c r="S6">
+        <v>16</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="9">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="AB6">
+        <v>2</v>
+      </c>
+      <c r="AG6" s="3"/>
+      <c r="AH6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F7">
+        <v>1863</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>187</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="R7">
+        <v>50</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="9">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="AB7">
+        <v>2</v>
+      </c>
+      <c r="AG7" s="3"/>
+      <c r="AH7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" t="s">
+        <v>215</v>
+      </c>
+      <c r="F8">
+        <v>1856</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="J8" t="s">
+        <v>187</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="P8">
+        <v>900</v>
+      </c>
+      <c r="AA8" s="9">
+        <v>15.1</v>
+      </c>
+      <c r="AB8">
+        <v>4</v>
+      </c>
+      <c r="AG8" s="3"/>
+      <c r="AH8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" t="s">
+        <v>216</v>
+      </c>
+      <c r="F9">
+        <v>1868</v>
+      </c>
+      <c r="J9" t="s">
+        <v>187</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="R9">
+        <v>100</v>
+      </c>
+      <c r="AA9" s="9">
+        <v>11.8</v>
+      </c>
+      <c r="AB9">
+        <v>2</v>
+      </c>
+      <c r="AG9" s="3"/>
+      <c r="AH9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" t="s">
+        <v>217</v>
+      </c>
+      <c r="J10" t="s">
+        <v>187</v>
+      </c>
+      <c r="AG10" s="3"/>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>186</v>
+      </c>
+      <c r="J11" t="s">
+        <v>187</v>
+      </c>
+      <c r="AG11" s="3"/>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>186</v>
+      </c>
+      <c r="J12" t="s">
+        <v>187</v>
+      </c>
+      <c r="AG12" s="3"/>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>186</v>
+      </c>
+      <c r="J13" t="s">
+        <v>187</v>
+      </c>
+      <c r="AG13" s="3"/>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>186</v>
+      </c>
+      <c r="J14" t="s">
+        <v>187</v>
+      </c>
+      <c r="AG14" s="3"/>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>186</v>
+      </c>
+      <c r="J15" t="s">
+        <v>187</v>
+      </c>
+      <c r="AG15" s="3"/>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>186</v>
+      </c>
+      <c r="J16" t="s">
+        <v>187</v>
+      </c>
+      <c r="AG16" s="3"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>186</v>
+      </c>
+      <c r="J17" t="s">
+        <v>187</v>
+      </c>
+      <c r="AG17" s="3"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>186</v>
+      </c>
+      <c r="J18" t="s">
+        <v>187</v>
+      </c>
+      <c r="AG18" s="3"/>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG19" s="3"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG20" s="3"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG21" s="3"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG22" s="3"/>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG23" s="3"/>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG24" s="3"/>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG25" s="3"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG26" s="3"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG27" s="3"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG28" s="3"/>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG29" s="3"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG30" s="3"/>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG31" s="3"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG32" s="3"/>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG33" s="3"/>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG34" s="3"/>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG35" s="3"/>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG36" s="3"/>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG37" s="3"/>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG38" s="3"/>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG39" s="3"/>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG40" s="3"/>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG41" s="3"/>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG42" s="3"/>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG43" s="3"/>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG44" s="3"/>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG45" s="3"/>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG46" s="3"/>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG47" s="3"/>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG48" s="3"/>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG49" s="3"/>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG50" s="3"/>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG51" s="3"/>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG52" s="3"/>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG53" s="3"/>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG54" s="3"/>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG55" s="3"/>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG56" s="3"/>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG57" s="3"/>
+    </row>
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG58" s="3"/>
+    </row>
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG59" s="3"/>
+    </row>
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG60" s="3"/>
+    </row>
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG61" s="3"/>
+    </row>
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG62" s="3"/>
+    </row>
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG63" s="3"/>
+    </row>
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG64" s="3"/>
+    </row>
+    <row r="65" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG65" s="3"/>
+    </row>
+    <row r="66" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG66" s="3"/>
+    </row>
+    <row r="67" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG67" s="3"/>
+    </row>
+    <row r="68" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG68" s="3"/>
+    </row>
+    <row r="69" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG69" s="3"/>
+    </row>
+    <row r="70" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG70" s="3"/>
+    </row>
+    <row r="71" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG71" s="3"/>
+    </row>
+    <row r="72" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG72" s="3"/>
+    </row>
+    <row r="73" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG73" s="3"/>
+    </row>
+    <row r="74" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG74" s="3"/>
+    </row>
+    <row r="75" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG75" s="3"/>
+    </row>
+    <row r="76" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG76" s="3"/>
+    </row>
+    <row r="77" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG77" s="3"/>
+    </row>
+    <row r="78" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG78" s="3"/>
+    </row>
+    <row r="79" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG79" s="3"/>
+    </row>
+    <row r="80" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG80" s="3"/>
+    </row>
+    <row r="81" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG81" s="3"/>
+    </row>
+    <row r="82" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG82" s="3"/>
+    </row>
+    <row r="83" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG83" s="3"/>
+    </row>
+    <row r="84" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG84" s="3"/>
+    </row>
+    <row r="85" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG85" s="3"/>
+    </row>
+    <row r="86" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG86" s="3"/>
+    </row>
+    <row r="87" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG87" s="3"/>
+    </row>
+    <row r="88" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG88" s="3"/>
+    </row>
+    <row r="89" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG89" s="3"/>
+    </row>
+    <row r="90" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG90" s="3"/>
+    </row>
+    <row r="91" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG91" s="3"/>
+    </row>
+    <row r="92" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG92" s="3"/>
+    </row>
+    <row r="93" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG93" s="3"/>
+    </row>
+    <row r="94" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG94" s="3"/>
+    </row>
+    <row r="95" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG95" s="3"/>
+    </row>
+    <row r="96" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG96" s="3"/>
+    </row>
+    <row r="97" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG97" s="3"/>
+    </row>
+    <row r="98" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG98" s="3"/>
+    </row>
+    <row r="99" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG99" s="3"/>
+    </row>
+    <row r="100" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG100" s="3"/>
+    </row>
+    <row r="101" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG101" s="3"/>
+    </row>
+    <row r="102" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG102" s="3"/>
+    </row>
+    <row r="103" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG103" s="3"/>
+    </row>
+    <row r="104" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG104" s="3"/>
+    </row>
+    <row r="105" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG105" s="3"/>
+    </row>
+    <row r="106" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG106" s="3"/>
+    </row>
+    <row r="107" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG107" s="3"/>
+    </row>
+    <row r="108" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG108" s="3"/>
+    </row>
+    <row r="109" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG109" s="3"/>
+    </row>
+    <row r="110" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG110" s="3"/>
+    </row>
+    <row r="111" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG111" s="3"/>
+    </row>
+    <row r="112" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG112" s="3"/>
+    </row>
+    <row r="113" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG113" s="3"/>
+    </row>
+    <row r="114" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG114" s="3"/>
+    </row>
+    <row r="115" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG115" s="3"/>
+    </row>
+    <row r="116" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG116" s="3"/>
+    </row>
+    <row r="117" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG117" s="3"/>
+    </row>
+    <row r="118" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG118" s="3"/>
+    </row>
+    <row r="119" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG119" s="3"/>
+    </row>
+    <row r="120" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG120" s="3"/>
+    </row>
+    <row r="121" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG121" s="3"/>
+    </row>
+    <row r="122" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG122" s="3"/>
+    </row>
+    <row r="123" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG123" s="3"/>
+    </row>
+    <row r="124" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG124" s="3"/>
+    </row>
+    <row r="125" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG125" s="3"/>
+    </row>
+    <row r="126" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG126" s="3"/>
+    </row>
+    <row r="127" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG127" s="3"/>
+    </row>
+    <row r="128" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG128" s="3"/>
+    </row>
+    <row r="129" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG129" s="3"/>
+    </row>
+    <row r="130" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG130" s="3"/>
+    </row>
+    <row r="131" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG131" s="3"/>
+    </row>
+    <row r="132" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG132" s="3"/>
+    </row>
+    <row r="133" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG133" s="3"/>
+    </row>
+    <row r="134" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG134" s="3"/>
+    </row>
+    <row r="135" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG135" s="3"/>
+    </row>
+    <row r="136" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG136" s="3"/>
+    </row>
+    <row r="137" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG137" s="3"/>
+    </row>
+    <row r="138" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG138" s="3"/>
+    </row>
+    <row r="139" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG139" s="3"/>
+    </row>
+    <row r="140" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG140" s="3"/>
+    </row>
+    <row r="141" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG141" s="3"/>
+    </row>
+    <row r="142" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG142" s="3"/>
+    </row>
+    <row r="143" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG143" s="3"/>
+    </row>
+    <row r="144" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG144" s="3"/>
+    </row>
+    <row r="145" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG145" s="3"/>
+    </row>
+    <row r="146" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG146" s="3"/>
+    </row>
+    <row r="147" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG147" s="3"/>
+    </row>
+    <row r="148" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG148" s="3"/>
+    </row>
+    <row r="149" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG149" s="3"/>
+    </row>
+    <row r="150" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG150" s="3"/>
+    </row>
+    <row r="151" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG151" s="3"/>
+    </row>
+    <row r="152" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG152" s="3"/>
+    </row>
+    <row r="153" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG153" s="3"/>
+    </row>
+    <row r="154" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG154" s="3"/>
+    </row>
+    <row r="155" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG155" s="3"/>
+    </row>
+    <row r="156" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG156" s="3"/>
+    </row>
+    <row r="157" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG157" s="3"/>
+    </row>
+    <row r="158" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG158" s="3"/>
+    </row>
+    <row r="159" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG159" s="3"/>
+    </row>
+    <row r="160" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG160" s="3"/>
+    </row>
+    <row r="161" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG161" s="3"/>
+    </row>
+    <row r="162" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG162" s="3"/>
+    </row>
+    <row r="163" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG163" s="3"/>
+    </row>
+    <row r="164" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG164" s="3"/>
+    </row>
+    <row r="165" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG165" s="3"/>
+    </row>
+    <row r="166" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG166" s="3"/>
+    </row>
+    <row r="167" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG167" s="3"/>
+    </row>
+    <row r="168" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG168" s="3"/>
+    </row>
+    <row r="169" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG169" s="3"/>
+    </row>
+    <row r="170" spans="33:33" x14ac:dyDescent="0.25">
+      <c r="AG170" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1588DABD-649C-440E-B3E7-F4DCE1430BE3}">
+  <dimension ref="A1:AZ170"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="9.140625" style="8"/>
+    <col min="32" max="32" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>193</v>
+      </c>
       <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" t="s">
-        <v>95</v>
-      </c>
       <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>45</v>
       </c>
-      <c r="L1" t="s">
-        <v>81</v>
-      </c>
       <c r="M1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N1" t="s">
+        <v>80</v>
+      </c>
+      <c r="O1" t="s">
         <v>46</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="S1" t="s">
         <v>47</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="U1" t="s">
+        <v>189</v>
+      </c>
+      <c r="V1" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="W1" t="s">
         <v>49</v>
       </c>
-      <c r="R1" t="s">
+      <c r="X1" t="s">
         <v>50</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Y1" t="s">
         <v>51</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Z1" t="s">
         <v>52</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AA1" t="s">
         <v>53</v>
       </c>
-      <c r="V1" t="s">
-        <v>92</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="AB1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC1" t="s">
         <v>54</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AD1" t="s">
         <v>55</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AE1" t="s">
         <v>56</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AF1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AG1" t="s">
         <v>58</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AH1" t="s">
         <v>59</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AI1" t="s">
         <v>60</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AJ1" t="s">
         <v>61</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AK1" t="s">
         <v>62</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AL1" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AN1" t="s">
         <v>63</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AO1" t="s">
         <v>64</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AP1" t="s">
         <v>65</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AQ1" t="s">
         <v>66</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AR1" t="s">
         <v>67</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AS1" t="s">
         <v>68</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AT1" t="s">
         <v>69</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AU1" t="s">
         <v>70</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AV1" t="s">
         <v>71</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AW1" t="s">
         <v>72</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AX1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY1" t="s">
         <v>74</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AZ1" t="s">
         <v>75</v>
       </c>
-      <c r="AR1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>73</v>
-      </c>
+    </row>
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F2" s="8">
+        <v>50</v>
+      </c>
+      <c r="K2">
+        <v>1847</v>
+      </c>
+      <c r="L2">
+        <v>6</v>
+      </c>
+      <c r="O2" t="s">
+        <v>187</v>
+      </c>
+      <c r="S2" s="1"/>
+      <c r="AF2" s="9">
+        <v>20</v>
+      </c>
+      <c r="AG2">
+        <v>3</v>
+      </c>
+      <c r="AL2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F3" s="8">
+        <v>50</v>
+      </c>
+      <c r="K3">
+        <v>1847</v>
+      </c>
+      <c r="L3">
+        <v>6</v>
+      </c>
+      <c r="O3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AF3" s="9">
+        <v>21</v>
+      </c>
+      <c r="AG3">
+        <v>3</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D4" t="s">
+        <v>203</v>
+      </c>
+      <c r="K4">
+        <v>1856</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="O4" t="s">
+        <v>187</v>
+      </c>
+      <c r="AF4" s="9">
+        <v>28.8</v>
+      </c>
+      <c r="AG4">
+        <v>3</v>
+      </c>
+      <c r="AL4">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" t="s">
+        <v>206</v>
+      </c>
+      <c r="K5">
+        <v>1856</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="O5" t="s">
+        <v>187</v>
+      </c>
+      <c r="AF5" s="9">
+        <v>29</v>
+      </c>
+      <c r="AG5">
+        <v>3</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" t="s">
+        <v>208</v>
+      </c>
+      <c r="K6">
+        <v>1856</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="O6" t="s">
+        <v>187</v>
+      </c>
+      <c r="AF6" s="9">
+        <v>29.5</v>
+      </c>
+      <c r="AG6">
+        <v>3</v>
+      </c>
+      <c r="AL6">
+        <v>1</v>
+      </c>
+      <c r="AM6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" t="s">
+        <v>208</v>
+      </c>
+      <c r="K7">
+        <v>1856</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="O7" t="s">
+        <v>187</v>
+      </c>
+      <c r="AF7" s="9">
+        <v>25.9</v>
+      </c>
+      <c r="AG7">
+        <v>3</v>
+      </c>
+      <c r="AL7">
+        <v>1</v>
+      </c>
+      <c r="AM7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" t="s">
+        <v>208</v>
+      </c>
+      <c r="K8">
+        <v>1858</v>
+      </c>
+      <c r="L8" t="s">
+        <v>213</v>
+      </c>
+      <c r="O8" t="s">
+        <v>187</v>
+      </c>
+      <c r="AF8" s="9">
+        <v>22.6</v>
+      </c>
+      <c r="AG8">
+        <v>3</v>
+      </c>
+      <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AM8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" t="s">
+        <v>212</v>
+      </c>
+      <c r="K9">
+        <v>1858</v>
+      </c>
+      <c r="L9" t="s">
+        <v>213</v>
+      </c>
+      <c r="O9" t="s">
+        <v>187</v>
+      </c>
+      <c r="AF9" s="9">
+        <v>27.7</v>
+      </c>
+      <c r="AG9">
+        <v>3</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" t="s">
+        <v>208</v>
+      </c>
+      <c r="F10" s="8">
+        <v>100</v>
+      </c>
+      <c r="O10" t="s">
+        <v>187</v>
+      </c>
+      <c r="AM10" s="3"/>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>186</v>
+      </c>
+      <c r="O11" t="s">
+        <v>187</v>
+      </c>
+      <c r="AM11" s="3"/>
+    </row>
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>186</v>
+      </c>
+      <c r="O12" t="s">
+        <v>187</v>
+      </c>
+      <c r="AM12" s="3"/>
+    </row>
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O13" t="s">
+        <v>187</v>
+      </c>
+      <c r="AM13" s="3"/>
+    </row>
+    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>186</v>
+      </c>
+      <c r="O14" t="s">
+        <v>187</v>
+      </c>
+      <c r="AM14" s="3"/>
+    </row>
+    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>186</v>
+      </c>
+      <c r="O15" t="s">
+        <v>187</v>
+      </c>
+      <c r="AM15" s="3"/>
+    </row>
+    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O16" t="s">
+        <v>187</v>
+      </c>
+      <c r="AM16" s="3"/>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>186</v>
+      </c>
+      <c r="O17" t="s">
+        <v>187</v>
+      </c>
+      <c r="AM17" s="3"/>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>186</v>
+      </c>
+      <c r="O18" t="s">
+        <v>187</v>
+      </c>
+      <c r="AM18" s="3"/>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM19" s="3"/>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM20" s="3"/>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM21" s="3"/>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM22" s="3"/>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM23" s="3"/>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM24" s="3"/>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM25" s="3"/>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM26" s="3"/>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM27" s="3"/>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM28" s="3"/>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM29" s="3"/>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM30" s="3"/>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM31" s="3"/>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM32" s="3"/>
+    </row>
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM33" s="3"/>
+    </row>
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM34" s="3"/>
+    </row>
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM35" s="3"/>
+    </row>
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM36" s="3"/>
+    </row>
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM37" s="3"/>
+    </row>
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM38" s="3"/>
+    </row>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM39" s="3"/>
+    </row>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM40" s="3"/>
+    </row>
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM41" s="3"/>
+    </row>
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM42" s="3"/>
+    </row>
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM43" s="3"/>
+    </row>
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM44" s="3"/>
+    </row>
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM45" s="3"/>
+    </row>
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM46" s="3"/>
+    </row>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM47" s="3"/>
+    </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM48" s="3"/>
+    </row>
+    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM49" s="3"/>
+    </row>
+    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM50" s="3"/>
+    </row>
+    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM51" s="3"/>
+    </row>
+    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM52" s="3"/>
+    </row>
+    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM53" s="3"/>
+    </row>
+    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM54" s="3"/>
+    </row>
+    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM55" s="3"/>
+    </row>
+    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM56" s="3"/>
+    </row>
+    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM57" s="3"/>
+    </row>
+    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM58" s="3"/>
+    </row>
+    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM59" s="3"/>
+    </row>
+    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM60" s="3"/>
+    </row>
+    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM61" s="3"/>
+    </row>
+    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM62" s="3"/>
+    </row>
+    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM63" s="3"/>
+    </row>
+    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM64" s="3"/>
+    </row>
+    <row r="65" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM65" s="3"/>
+    </row>
+    <row r="66" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM66" s="3"/>
+    </row>
+    <row r="67" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM67" s="3"/>
+    </row>
+    <row r="68" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM68" s="3"/>
+    </row>
+    <row r="69" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM69" s="3"/>
+    </row>
+    <row r="70" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM70" s="3"/>
+    </row>
+    <row r="71" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM71" s="3"/>
+    </row>
+    <row r="72" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM72" s="3"/>
+    </row>
+    <row r="73" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM73" s="3"/>
+    </row>
+    <row r="74" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM74" s="3"/>
+    </row>
+    <row r="75" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM75" s="3"/>
+    </row>
+    <row r="76" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM76" s="3"/>
+    </row>
+    <row r="77" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM77" s="3"/>
+    </row>
+    <row r="78" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM78" s="3"/>
+    </row>
+    <row r="79" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM79" s="3"/>
+    </row>
+    <row r="80" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM80" s="3"/>
+    </row>
+    <row r="81" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM81" s="3"/>
+    </row>
+    <row r="82" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM82" s="3"/>
+    </row>
+    <row r="83" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM83" s="3"/>
+    </row>
+    <row r="84" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM84" s="3"/>
+    </row>
+    <row r="85" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM85" s="3"/>
+    </row>
+    <row r="86" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM86" s="3"/>
+    </row>
+    <row r="87" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM87" s="3"/>
+    </row>
+    <row r="88" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM88" s="3"/>
+    </row>
+    <row r="89" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM89" s="3"/>
+    </row>
+    <row r="90" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM90" s="3"/>
+    </row>
+    <row r="91" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM91" s="3"/>
+    </row>
+    <row r="92" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM92" s="3"/>
+    </row>
+    <row r="93" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM93" s="3"/>
+    </row>
+    <row r="94" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM94" s="3"/>
+    </row>
+    <row r="95" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM95" s="3"/>
+    </row>
+    <row r="96" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM96" s="3"/>
+    </row>
+    <row r="97" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM97" s="3"/>
+    </row>
+    <row r="98" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM98" s="3"/>
+    </row>
+    <row r="99" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM99" s="3"/>
+    </row>
+    <row r="100" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM100" s="3"/>
+    </row>
+    <row r="101" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM101" s="3"/>
+    </row>
+    <row r="102" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM102" s="3"/>
+    </row>
+    <row r="103" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM103" s="3"/>
+    </row>
+    <row r="104" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM104" s="3"/>
+    </row>
+    <row r="105" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM105" s="3"/>
+    </row>
+    <row r="106" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM106" s="3"/>
+    </row>
+    <row r="107" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM107" s="3"/>
+    </row>
+    <row r="108" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM108" s="3"/>
+    </row>
+    <row r="109" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM109" s="3"/>
+    </row>
+    <row r="110" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM110" s="3"/>
+    </row>
+    <row r="111" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM111" s="3"/>
+    </row>
+    <row r="112" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM112" s="3"/>
+    </row>
+    <row r="113" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM113" s="3"/>
+    </row>
+    <row r="114" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM114" s="3"/>
+    </row>
+    <row r="115" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM115" s="3"/>
+    </row>
+    <row r="116" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM116" s="3"/>
+    </row>
+    <row r="117" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM117" s="3"/>
+    </row>
+    <row r="118" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM118" s="3"/>
+    </row>
+    <row r="119" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM119" s="3"/>
+    </row>
+    <row r="120" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM120" s="3"/>
+    </row>
+    <row r="121" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM121" s="3"/>
+    </row>
+    <row r="122" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM122" s="3"/>
+    </row>
+    <row r="123" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM123" s="3"/>
+    </row>
+    <row r="124" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM124" s="3"/>
+    </row>
+    <row r="125" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM125" s="3"/>
+    </row>
+    <row r="126" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM126" s="3"/>
+    </row>
+    <row r="127" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM127" s="3"/>
+    </row>
+    <row r="128" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM128" s="3"/>
+    </row>
+    <row r="129" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM129" s="3"/>
+    </row>
+    <row r="130" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM130" s="3"/>
+    </row>
+    <row r="131" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM131" s="3"/>
+    </row>
+    <row r="132" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM132" s="3"/>
+    </row>
+    <row r="133" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM133" s="3"/>
+    </row>
+    <row r="134" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM134" s="3"/>
+    </row>
+    <row r="135" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM135" s="3"/>
+    </row>
+    <row r="136" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM136" s="3"/>
+    </row>
+    <row r="137" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM137" s="3"/>
+    </row>
+    <row r="138" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM138" s="3"/>
+    </row>
+    <row r="139" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM139" s="3"/>
+    </row>
+    <row r="140" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM140" s="3"/>
+    </row>
+    <row r="141" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM141" s="3"/>
+    </row>
+    <row r="142" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM142" s="3"/>
+    </row>
+    <row r="143" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM143" s="3"/>
+    </row>
+    <row r="144" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM144" s="3"/>
+    </row>
+    <row r="145" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM145" s="3"/>
+    </row>
+    <row r="146" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM146" s="3"/>
+    </row>
+    <row r="147" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM147" s="3"/>
+    </row>
+    <row r="148" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM148" s="3"/>
+    </row>
+    <row r="149" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM149" s="3"/>
+    </row>
+    <row r="150" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM150" s="3"/>
+    </row>
+    <row r="151" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM151" s="3"/>
+    </row>
+    <row r="152" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM152" s="3"/>
+    </row>
+    <row r="153" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM153" s="3"/>
+    </row>
+    <row r="154" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM154" s="3"/>
+    </row>
+    <row r="155" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM155" s="3"/>
+    </row>
+    <row r="156" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM156" s="3"/>
+    </row>
+    <row r="157" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM157" s="3"/>
+    </row>
+    <row r="158" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM158" s="3"/>
+    </row>
+    <row r="159" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM159" s="3"/>
+    </row>
+    <row r="160" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM160" s="3"/>
+    </row>
+    <row r="161" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM161" s="3"/>
+    </row>
+    <row r="162" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM162" s="3"/>
+    </row>
+    <row r="163" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM163" s="3"/>
+    </row>
+    <row r="164" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM164" s="3"/>
+    </row>
+    <row r="165" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM165" s="3"/>
+    </row>
+    <row r="166" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM166" s="3"/>
+    </row>
+    <row r="167" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM167" s="3"/>
+    </row>
+    <row r="168" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM168" s="3"/>
+    </row>
+    <row r="169" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM169" s="3"/>
+    </row>
+    <row r="170" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM170" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>